<commit_message>
now works with familiarisation area
</commit_message>
<xml_diff>
--- a/Example Notebooks/custom_assignments_test.xlsx
+++ b/Example Notebooks/custom_assignments_test.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\padin_000\Documents\github\qub_canvas_helper\Example Notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Dingwall\Documents\github\qub_canvas_helper\qub_canvas_helper\Example Notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E93054-F752-400D-8C27-0E7A085CFE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6935A234-63B7-4A32-840A-5A3E21AC5A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -52,6 +63,21 @@
   </si>
   <si>
     <t>Notareal Person</t>
+  </si>
+  <si>
+    <t>FA_Student2</t>
+  </si>
+  <si>
+    <t>FA_Student3</t>
+  </si>
+  <si>
+    <t>FA_Student4</t>
+  </si>
+  <si>
+    <t>FA_Student5</t>
+  </si>
+  <si>
+    <t>FA_Student6</t>
   </si>
 </sst>
 </file>
@@ -73,12 +99,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,12 +125,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,20 +415,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H14:H15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,15 +437,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1">
-        <v>45589</v>
+        <v>45649</v>
       </c>
       <c r="D1" s="1">
-        <v>45597</v>
+        <v>45656</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1491</v>
+    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -419,10 +456,12 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>1490</v>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -433,10 +472,12 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>1492</v>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -447,10 +488,12 @@
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>1493</v>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -461,10 +504,12 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="33" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>45</v>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -475,6 +520,8 @@
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>